<commit_message>
Successfully copied over emails, now just have to delete empty rows
</commit_message>
<xml_diff>
--- a/MailMerge.xlsx
+++ b/MailMerge.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python36-32\Python Scripts\Mail Merge App\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="1077">
   <si>
     <t>OSC Number</t>
   </si>
@@ -3250,20 +3255,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -3279,15 +3283,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3575,20 +3588,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="E189" sqref="C2:E189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +3639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3649,7 +3665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3675,7 +3691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -3701,7 +3717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -3727,7 +3743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3753,7 +3769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -3779,7 +3795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -3805,7 +3821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -3831,7 +3847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3857,7 +3873,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -3883,7 +3899,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -3909,7 +3925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -3935,7 +3951,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>88</v>
       </c>
@@ -3961,7 +3977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -3987,7 +4003,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -4013,7 +4029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>106</v>
       </c>
@@ -4039,7 +4055,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -4065,7 +4081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -4091,7 +4107,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -4117,7 +4133,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -4143,7 +4159,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -4169,7 +4185,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -4195,7 +4211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -4221,7 +4237,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -4247,7 +4263,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -4273,7 +4289,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>165</v>
       </c>
@@ -4299,7 +4315,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>171</v>
       </c>
@@ -4325,7 +4341,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>177</v>
       </c>
@@ -4351,7 +4367,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>183</v>
       </c>
@@ -4377,7 +4393,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>189</v>
       </c>
@@ -4403,7 +4419,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>195</v>
       </c>
@@ -4429,7 +4445,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>200</v>
       </c>
@@ -4455,7 +4471,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>206</v>
       </c>
@@ -4481,7 +4497,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>212</v>
       </c>
@@ -4507,7 +4523,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>218</v>
       </c>
@@ -4533,7 +4549,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>224</v>
       </c>
@@ -4559,7 +4575,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>230</v>
       </c>
@@ -4585,7 +4601,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>235</v>
       </c>
@@ -4611,7 +4627,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>241</v>
       </c>
@@ -4637,7 +4653,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>246</v>
       </c>
@@ -4663,7 +4679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>252</v>
       </c>
@@ -4689,7 +4705,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>257</v>
       </c>
@@ -4715,7 +4731,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>263</v>
       </c>
@@ -4741,7 +4757,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>269</v>
       </c>
@@ -4767,7 +4783,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>275</v>
       </c>
@@ -4793,7 +4809,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>281</v>
       </c>
@@ -4819,7 +4835,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>287</v>
       </c>
@@ -4845,7 +4861,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>293</v>
       </c>
@@ -4871,7 +4887,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>299</v>
       </c>
@@ -4897,7 +4913,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>304</v>
       </c>
@@ -4923,7 +4939,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>310</v>
       </c>
@@ -4949,7 +4965,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>315</v>
       </c>
@@ -4975,7 +4991,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>320</v>
       </c>
@@ -5001,7 +5017,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>326</v>
       </c>
@@ -5027,7 +5043,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>331</v>
       </c>
@@ -5053,7 +5069,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>337</v>
       </c>
@@ -5079,7 +5095,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>343</v>
       </c>
@@ -5105,7 +5121,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>349</v>
       </c>
@@ -5131,7 +5147,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>354</v>
       </c>
@@ -5157,7 +5173,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>360</v>
       </c>
@@ -5183,7 +5199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>365</v>
       </c>
@@ -5209,7 +5225,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>371</v>
       </c>
@@ -5235,7 +5251,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>376</v>
       </c>
@@ -5261,7 +5277,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>382</v>
       </c>
@@ -5287,7 +5303,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>388</v>
       </c>
@@ -5313,7 +5329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>394</v>
       </c>
@@ -5339,7 +5355,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>400</v>
       </c>
@@ -5365,7 +5381,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>406</v>
       </c>
@@ -5391,7 +5407,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>412</v>
       </c>
@@ -5417,7 +5433,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>417</v>
       </c>
@@ -5443,7 +5459,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>423</v>
       </c>
@@ -5469,7 +5485,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>429</v>
       </c>
@@ -5495,7 +5511,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>435</v>
       </c>
@@ -5521,7 +5537,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>441</v>
       </c>
@@ -5547,7 +5563,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>447</v>
       </c>
@@ -5573,7 +5589,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>453</v>
       </c>
@@ -5599,7 +5615,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>459</v>
       </c>
@@ -5625,7 +5641,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>465</v>
       </c>
@@ -5651,7 +5667,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>471</v>
       </c>
@@ -5677,7 +5693,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>477</v>
       </c>
@@ -5703,7 +5719,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>483</v>
       </c>
@@ -5729,7 +5745,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>489</v>
       </c>
@@ -5755,7 +5771,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>495</v>
       </c>
@@ -5781,7 +5797,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>500</v>
       </c>
@@ -5807,7 +5823,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>506</v>
       </c>
@@ -5833,7 +5849,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>512</v>
       </c>
@@ -5859,7 +5875,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>518</v>
       </c>
@@ -5885,7 +5901,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>523</v>
       </c>
@@ -5911,7 +5927,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>529</v>
       </c>
@@ -5937,7 +5953,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>535</v>
       </c>
@@ -5963,7 +5979,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>541</v>
       </c>
@@ -5989,7 +6005,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>547</v>
       </c>
@@ -6015,7 +6031,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>553</v>
       </c>
@@ -6041,7 +6057,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>559</v>
       </c>
@@ -6067,7 +6083,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>564</v>
       </c>
@@ -6093,7 +6109,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>570</v>
       </c>
@@ -6119,7 +6135,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>576</v>
       </c>
@@ -6145,7 +6161,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>582</v>
       </c>
@@ -6171,7 +6187,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>588</v>
       </c>
@@ -6197,7 +6213,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>594</v>
       </c>
@@ -6223,7 +6239,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>600</v>
       </c>
@@ -6249,7 +6265,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>606</v>
       </c>
@@ -6275,7 +6291,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>611</v>
       </c>
@@ -6301,7 +6317,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>617</v>
       </c>
@@ -6327,7 +6343,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>623</v>
       </c>
@@ -6353,7 +6369,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>629</v>
       </c>
@@ -6379,7 +6395,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>635</v>
       </c>
@@ -6405,7 +6421,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>640</v>
       </c>
@@ -6431,7 +6447,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>646</v>
       </c>
@@ -6457,7 +6473,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>649</v>
       </c>
@@ -6483,7 +6499,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>654</v>
       </c>
@@ -6509,7 +6525,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>660</v>
       </c>
@@ -6535,7 +6551,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>663</v>
       </c>
@@ -6561,7 +6577,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>669</v>
       </c>
@@ -6587,7 +6603,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>672</v>
       </c>
@@ -6613,7 +6629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>678</v>
       </c>
@@ -6639,7 +6655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>684</v>
       </c>
@@ -6665,7 +6681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>689</v>
       </c>
@@ -6691,7 +6707,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>694</v>
       </c>
@@ -6717,7 +6733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>700</v>
       </c>
@@ -6743,7 +6759,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>706</v>
       </c>
@@ -6769,7 +6785,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>711</v>
       </c>
@@ -6795,7 +6811,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>716</v>
       </c>
@@ -6821,7 +6837,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>721</v>
       </c>
@@ -6847,7 +6863,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>727</v>
       </c>
@@ -6873,7 +6889,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>733</v>
       </c>
@@ -6899,7 +6915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>739</v>
       </c>
@@ -6925,7 +6941,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>744</v>
       </c>
@@ -6951,7 +6967,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>750</v>
       </c>
@@ -6977,7 +6993,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>756</v>
       </c>
@@ -7003,7 +7019,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>762</v>
       </c>
@@ -7029,7 +7045,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>767</v>
       </c>
@@ -7055,7 +7071,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>772</v>
       </c>
@@ -7081,7 +7097,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>777</v>
       </c>
@@ -7107,7 +7123,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>782</v>
       </c>
@@ -7133,7 +7149,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>787</v>
       </c>
@@ -7159,7 +7175,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>793</v>
       </c>
@@ -7185,7 +7201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>799</v>
       </c>
@@ -7211,7 +7227,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>804</v>
       </c>
@@ -7237,7 +7253,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>810</v>
       </c>
@@ -7263,7 +7279,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>816</v>
       </c>
@@ -7289,7 +7305,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>821</v>
       </c>
@@ -7315,7 +7331,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>826</v>
       </c>
@@ -7341,7 +7357,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>831</v>
       </c>
@@ -7367,7 +7383,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>837</v>
       </c>
@@ -7393,7 +7409,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>840</v>
       </c>
@@ -7419,7 +7435,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>845</v>
       </c>
@@ -7445,7 +7461,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>851</v>
       </c>
@@ -7471,7 +7487,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>856</v>
       </c>
@@ -7497,7 +7513,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>862</v>
       </c>
@@ -7523,7 +7539,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>868</v>
       </c>
@@ -7549,7 +7565,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>874</v>
       </c>
@@ -7575,7 +7591,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>879</v>
       </c>
@@ -7601,7 +7617,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>883</v>
       </c>
@@ -7627,7 +7643,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>888</v>
       </c>
@@ -7653,7 +7669,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>894</v>
       </c>
@@ -7679,7 +7695,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>900</v>
       </c>
@@ -7705,7 +7721,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>906</v>
       </c>
@@ -7731,7 +7747,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>911</v>
       </c>
@@ -7757,7 +7773,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>916</v>
       </c>
@@ -7783,7 +7799,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>921</v>
       </c>
@@ -7809,7 +7825,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>926</v>
       </c>
@@ -7835,7 +7851,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>931</v>
       </c>
@@ -7861,7 +7877,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>936</v>
       </c>
@@ -7887,7 +7903,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>941</v>
       </c>
@@ -7913,7 +7929,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>947</v>
       </c>
@@ -7939,7 +7955,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>953</v>
       </c>
@@ -7965,7 +7981,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>959</v>
       </c>
@@ -7991,7 +8007,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>965</v>
       </c>
@@ -8017,7 +8033,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>970</v>
       </c>
@@ -8043,7 +8059,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>975</v>
       </c>
@@ -8069,7 +8085,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>981</v>
       </c>
@@ -8095,7 +8111,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>987</v>
       </c>
@@ -8121,7 +8137,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>991</v>
       </c>
@@ -8147,7 +8163,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>997</v>
       </c>
@@ -8173,7 +8189,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>1002</v>
       </c>
@@ -8199,7 +8215,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>1007</v>
       </c>
@@ -8225,7 +8241,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>1012</v>
       </c>
@@ -8251,7 +8267,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>1018</v>
       </c>
@@ -8277,7 +8293,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>1024</v>
       </c>
@@ -8303,7 +8319,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>1030</v>
       </c>
@@ -8329,7 +8345,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>1036</v>
       </c>
@@ -8355,7 +8371,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>1041</v>
       </c>
@@ -8381,7 +8397,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>1046</v>
       </c>
@@ -8407,7 +8423,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>1049</v>
       </c>
@@ -8433,7 +8449,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>1054</v>
       </c>
@@ -8459,7 +8475,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>1059</v>
       </c>
@@ -8485,7 +8501,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>1065</v>
       </c>
@@ -8511,7 +8527,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>1071</v>
       </c>
@@ -8538,6 +8554,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>